<commit_message>
tRNA shuffling code, gene analysis (pull from EcoCyc)
</commit_message>
<xml_diff>
--- a/tRNAShuffle/bsub_codonValues.xlsx
+++ b/tRNAShuffle/bsub_codonValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshay/Documents/TranslationDynamics/tRNAShuffle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C29AE2F1-B6E7-6747-9B13-559AABA940FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C0A748-0F74-C54B-BBFD-A3DB0492886C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="59660" yWindow="1020" windowWidth="17920" windowHeight="21940" xr2:uid="{1F29E207-F7F4-F54D-B205-8792544E73B1}"/>
   </bookViews>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F7640C-3AFB-5343-9E5B-EB0359FD05F9}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>